<commit_message>
restore mpu and sd & fatfs
</commit_message>
<xml_diff>
--- a/Documents/CUAV_X7_PINOUT-2020-4-7.xlsx
+++ b/Documents/CUAV_X7_PINOUT-2020-4-7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22400" windowHeight="10210"/>
+    <workbookView windowWidth="18525" windowHeight="17670"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2155,11 +2155,11 @@
   <sheetPr/>
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D65" sqref="D62:D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21.375" customWidth="1"/>
     <col min="2" max="2" width="15.125" style="1" customWidth="1"/>

</xml_diff>